<commit_message>
se genera imagen comprobante
</commit_message>
<xml_diff>
--- a/ficha_final_cliente.xlsx
+++ b/ficha_final_cliente.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
   <si>
     <t>Fecha</t>
   </si>
@@ -43,47 +43,152 @@
     <t>04/03/23</t>
   </si>
   <si>
+    <t>05/03/23</t>
+  </si>
+  <si>
+    <t>06/03/23</t>
+  </si>
+  <si>
+    <t>07/03/23</t>
+  </si>
+  <si>
     <t>Marcelo Bader</t>
   </si>
   <si>
     <t>Marca Mattel</t>
   </si>
   <si>
+    <t>Tomás Gómez</t>
+  </si>
+  <si>
+    <t>Mär Es</t>
+  </si>
+  <si>
+    <t>Hans Peter</t>
+  </si>
+  <si>
+    <t>Linda Tarde</t>
+  </si>
+  <si>
+    <t>José Luis</t>
+  </si>
+  <si>
     <t>T206</t>
   </si>
   <si>
     <t>TEB308</t>
   </si>
   <si>
+    <t>TES824</t>
+  </si>
+  <si>
     <t>1234/4321</t>
   </si>
   <si>
     <t>180/4279</t>
   </si>
   <si>
+    <t>16293/672</t>
+  </si>
+  <si>
+    <t>2367/365</t>
+  </si>
+  <si>
+    <t>Fgg</t>
+  </si>
+  <si>
+    <t>162919/2718</t>
+  </si>
+  <si>
+    <t>1378/52</t>
+  </si>
+  <si>
+    <t>269201/361781</t>
+  </si>
+  <si>
+    <t>26817/71</t>
+  </si>
+  <si>
     <t>No enciende</t>
   </si>
   <si>
     <t>No tiene Ring</t>
   </si>
   <si>
+    <t>47391/262719</t>
+  </si>
+  <si>
+    <t>Ddf</t>
+  </si>
+  <si>
+    <t>No tiene tono en ext5</t>
+  </si>
+  <si>
     <t>Fusible y varistor de la fuente en corto</t>
   </si>
   <si>
     <t>Mosfet PWM defectuoso</t>
   </si>
   <si>
+    <t>Placa muy sulfatada</t>
+  </si>
+  <si>
+    <t>Ffg</t>
+  </si>
+  <si>
+    <t>Placa madre sulfatada</t>
+  </si>
+  <si>
+    <t>Supercapacitores en corto</t>
+  </si>
+  <si>
+    <t>Varistor en corto de ext5</t>
+  </si>
+  <si>
+    <t>Corto en bus de 3.3V</t>
+  </si>
+  <si>
     <t>Se cambia fusible y varistor</t>
   </si>
   <si>
     <t>Se cambia el Mosfet PWM</t>
+  </si>
+  <si>
+    <t>No tiene resolución</t>
+  </si>
+  <si>
+    <t>Jajaowo</t>
+  </si>
+  <si>
+    <t>Ffbb</t>
+  </si>
+  <si>
+    <t>Se cambian supercapacitores</t>
+  </si>
+  <si>
+    <t>Se cambia variator</t>
+  </si>
+  <si>
+    <t>No tiene resolución. No hay repuestos</t>
+  </si>
+  <si>
+    <t>S/C</t>
+  </si>
+  <si>
+    <t>Ddj</t>
+  </si>
+  <si>
+    <t>30000</t>
+  </si>
+  <si>
+    <t>15000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,16 +240,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -152,16 +251,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -235,7 +329,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -270,7 +363,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -446,101 +538,271 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="14" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="13.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="1">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="3">
-        <v>30000</v>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>